<commit_message>
add good creation functionality
</commit_message>
<xml_diff>
--- a/my_report.xlsx
+++ b/my_report.xlsx
@@ -1,31 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projects\beeline\SaryevaKlara_urok47\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D254DEBF-A222-411A-8D5E-CCA09827735D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF2DE196-3C32-457E-9942-E2F868F7A64F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-  </extLst>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>Компьютер</t>
   </si>
@@ -34,6 +29,9 @@
   </si>
   <si>
     <t>Мышка</t>
+  </si>
+  <si>
+    <t>Флаг</t>
   </si>
 </sst>
 </file>
@@ -351,11 +349,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:A4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -374,6 +370,11 @@
         <v>2</v>
       </c>
     </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>